<commit_message>
Made 'edit snippet' medium priority
</commit_message>
<xml_diff>
--- a/Documents/Storyboard.xlsx
+++ b/Documents/Storyboard.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
   <si>
     <t>Log In</t>
   </si>
@@ -316,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -334,12 +334,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -355,10 +349,20 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -667,443 +671,439 @@
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="9" customFormat="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:3" s="19" customFormat="1">
+      <c r="A1" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="9" customFormat="1"/>
-    <row r="3" spans="1:3" s="9" customFormat="1"/>
-    <row r="4" spans="1:3" s="9" customFormat="1"/>
-    <row r="5" spans="1:3">
-      <c r="A5" s="5" t="s">
+    <row r="2" spans="1:3" s="19" customFormat="1"/>
+    <row r="3" spans="1:3" s="19" customFormat="1"/>
+    <row r="4" spans="1:3" s="19" customFormat="1"/>
+    <row r="5" spans="1:3" s="23" customFormat="1"/>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="6" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="7" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="7" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="7" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="8"/>
-      <c r="B13" s="7" t="s">
-        <v>11</v>
+      <c r="B13" s="8"/>
+      <c r="C13" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="8"/>
-      <c r="B14" s="18"/>
+      <c r="B14" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="16"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="B20" s="12" t="s">
+    <row r="21" spans="1:3">
+      <c r="B21" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="B21" s="4" t="s">
+    <row r="22" spans="1:3">
+      <c r="B22" s="4" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="11"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
+      <c r="B24" s="9"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="2" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="B30" s="12" t="s">
+    <row r="31" spans="1:3">
+      <c r="B31" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="20" t="s">
+    <row r="51" spans="1:3">
+      <c r="A51" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="20"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="20"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="20"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="20"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="20"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="20"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B56" s="9"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15" customHeight="1">
+      <c r="A58" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15" customHeight="1">
+      <c r="A59" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15" customHeight="1">
+      <c r="A60" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15" customHeight="1">
+      <c r="C61" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="B62" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="B63" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="14" t="s">
+    <row r="66" spans="1:3">
+      <c r="A66" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1">
-      <c r="A40" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="15" t="s">
+    <row r="67" spans="1:3">
+      <c r="A67" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1">
-      <c r="A41" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="3" t="s">
+    <row r="68" spans="1:3">
+      <c r="A68" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1">
-      <c r="A42" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="3" t="s">
+    <row r="69" spans="1:3">
+      <c r="A69" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1">
-      <c r="B43" s="3" t="s">
+    <row r="70" spans="1:3" ht="15" customHeight="1">
+      <c r="A70" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="B70" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="C44" s="4" t="s">
+    <row r="71" spans="1:3">
+      <c r="B71" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="C45" s="4" t="s">
+    <row r="72" spans="1:3">
+      <c r="B72" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="B46" s="3" t="s">
+    <row r="73" spans="1:3">
+      <c r="A73" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="64.5">
-      <c r="A51" s="16" t="s">
+    <row r="76" spans="1:3" ht="64.5">
+      <c r="A76" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-    </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1">
-      <c r="A52" s="1" t="s">
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="14" t="s">
+    <row r="78" spans="1:3">
+      <c r="A78" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C78" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="3" t="s">
+    <row r="79" spans="1:3">
+      <c r="A79" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="3" t="s">
+    <row r="80" spans="1:3">
+      <c r="A80" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C80" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="3" t="s">
+    <row r="81" spans="1:3">
+      <c r="A81" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C81" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="3" t="s">
+    <row r="82" spans="1:3">
+      <c r="A82" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="3" t="s">
+    <row r="83" spans="1:3">
+      <c r="A83" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B58" s="11"/>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="1" t="s">
+      <c r="B83" s="9"/>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="14" t="s">
+    <row r="86" spans="1:3">
+      <c r="A86" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B86" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="3" t="s">
+    <row r="87" spans="1:3">
+      <c r="A87" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="3" t="s">
+    <row r="88" spans="1:3">
+      <c r="A88" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="3" t="s">
+    <row r="89" spans="1:3">
+      <c r="A89" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="3" t="s">
+    <row r="90" spans="1:3">
+      <c r="A90" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="3" t="s">
+    <row r="91" spans="1:3">
+      <c r="A91" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B66" s="11"/>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="B73" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="B77" s="11"/>
+      <c r="B91" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:XFD4"/>
-    <mergeCell ref="A33:C36"/>
+    <mergeCell ref="A51:C54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added description for final GUI tests of deliv3
</commit_message>
<xml_diff>
--- a/Documents/Storyboard.xlsx
+++ b/Documents/Storyboard.xlsx
@@ -81,12 +81,6 @@
     <t>Redirect to homepage</t>
   </si>
   <si>
-    <t xml:space="preserve"> Splice 1 (High Priority)</t>
-  </si>
-  <si>
-    <t>Splice 2 (Medium Priority)</t>
-  </si>
-  <si>
     <t>Delete snippet from codebox</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>Validate</t>
   </si>
   <si>
-    <t>Splice 3 (Low Priority)</t>
-  </si>
-  <si>
     <t>Group Management</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>Upload picture</t>
   </si>
   <si>
-    <t>Show groups for user</t>
-  </si>
-  <si>
     <t>Select group from list</t>
   </si>
   <si>
@@ -223,6 +211,18 @@
   </si>
   <si>
     <t>Add picture to user profile</t>
+  </si>
+  <si>
+    <t>Edit group</t>
+  </si>
+  <si>
+    <t>Slice 3 (Low Priority)</t>
+  </si>
+  <si>
+    <t>Slice 2 (Medium Priority)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slice 1 (High Priority)</t>
   </si>
 </sst>
 </file>
@@ -349,6 +349,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -359,10 +363,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -671,15 +671,15 @@
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="19" customFormat="1">
-      <c r="A1" s="18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="19" customFormat="1"/>
-    <row r="3" spans="1:3" s="19" customFormat="1"/>
-    <row r="4" spans="1:3" s="19" customFormat="1"/>
-    <row r="5" spans="1:3" s="23" customFormat="1"/>
+    <row r="1" spans="1:3" s="21" customFormat="1">
+      <c r="A1" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="21" customFormat="1"/>
+    <row r="3" spans="1:3" s="21" customFormat="1"/>
+    <row r="4" spans="1:3" s="21" customFormat="1"/>
+    <row r="5" spans="1:3" s="19" customFormat="1"/>
     <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
         <v>0</v>
@@ -698,10 +698,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -714,10 +714,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -775,7 +775,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
@@ -791,10 +791,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>16</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="B21" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -812,7 +812,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -828,61 +828,61 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" s="10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
+      <c r="A51" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="20"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="20"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="20"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
@@ -892,23 +892,23 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>6</v>
@@ -919,20 +919,20 @@
         <v>16</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" customHeight="1">
       <c r="C61" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="B62" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -942,34 +942,34 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B70" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="18" t="s">
         <v>8</v>
       </c>
     </row>
@@ -985,118 +985,118 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="64.5">
       <c r="A76" s="14" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C78" s="12" t="s">
-        <v>35</v>
+      <c r="C78" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B83" s="9"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B91" s="9"/>
     </row>

</xml_diff>